<commit_message>
Greedy heuristic with book moves
</commit_message>
<xml_diff>
--- a/wins.xlsx
+++ b/wins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernh\Documents\TU\7. Semester\SGP\MagicAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B2F680-ADDD-4B76-8366-725D60BCCD98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B568195C-21FA-437A-A525-AFAC43729193}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{214CF443-D217-4013-871E-FA22DACA3127}"/>
+    <workbookView xWindow="29295" yWindow="0" windowWidth="28305" windowHeight="15600" xr2:uid="{214CF443-D217-4013-871E-FA22DACA3127}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t>Player1</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Draws</t>
+  </si>
+  <si>
+    <t>Book Moves</t>
+  </si>
+  <si>
+    <t>P1Winrate</t>
+  </si>
+  <si>
+    <t>Greedy Book</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C564FCE0-9756-4245-84CB-0D37B64626E6}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +424,7 @@
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +440,11 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -448,8 +460,12 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>C2/(C2+D2)</f>
+        <v>0.69387755102040816</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -465,8 +481,12 @@
       <c r="E3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F12" si="0">C3/(C3+D3)</f>
+        <v>0.58904109589041098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -482,8 +502,12 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.55172413793103448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -499,8 +523,12 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -516,8 +544,12 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.73469387755102045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -532,6 +564,115 @@
       </c>
       <c r="E7">
         <v>3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.59863945578231292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>106</v>
+      </c>
+      <c r="D8">
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.54081632653061229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>94</v>
+      </c>
+      <c r="D10">
+        <v>55</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.63087248322147649</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>102</v>
+      </c>
+      <c r="D11">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.69863013698630139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>